<commit_message>
cell hien thi du lieu hoan thanh
</commit_message>
<xml_diff>
--- a/linux/view/customer.xlsx
+++ b/linux/view/customer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Dia chi</t>
+          <t>Dia diem</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -471,32 +471,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>k01</t>
+          <t>.!entry</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Nguyen Thien Thuat</t>
+          <t>.!combobox</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12/05/2001</t>
+          <t>.!entry2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>.!checkbutton1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Thanh Hoa</t>
+          <t>.!entry3</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0325258</t>
+          <t>.!spinbox</t>
         </is>
       </c>
     </row>
@@ -504,86 +504,16 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>k02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Trau Sinh Co</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>30/08/2003</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Nam</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Binh Dinh</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>025478008</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>k03</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Hoang Van Mau</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>14/02/2002</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Nu</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Dong Thap</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>0528475625</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>k04</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+          <t>.!checkbutton2</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>